<commit_message>
update YAML for mandatory fields
</commit_message>
<xml_diff>
--- a/docs/Mapping_Frontend_Backend.xlsx
+++ b/docs/Mapping_Frontend_Backend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parak\Documents\Parakram\astro_project\astro_aspects\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1589FA99-FADE-4810-9534-716A01B9F921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C306B280-0881-41A6-8EB9-6CB0135979B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{7B6B54E3-18D2-4A3E-8A3B-B1268B17FAEA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="215">
   <si>
     <t>Page</t>
   </si>
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F856F527-2095-420F-8F98-1B5B9DCBA563}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2158,9 +2158,6 @@
       <c r="D27" t="s">
         <v>58</v>
       </c>
-      <c r="F27" t="s">
-        <v>34</v>
-      </c>
       <c r="G27" t="s">
         <v>203</v>
       </c>
@@ -2181,9 +2178,6 @@
       <c r="D28" t="s">
         <v>56</v>
       </c>
-      <c r="F28" t="s">
-        <v>34</v>
-      </c>
       <c r="G28" t="s">
         <v>203</v>
       </c>
@@ -2204,9 +2198,6 @@
       <c r="D29" t="s">
         <v>56</v>
       </c>
-      <c r="F29" t="s">
-        <v>34</v>
-      </c>
       <c r="G29" t="s">
         <v>203</v>
       </c>
@@ -2227,9 +2218,6 @@
       <c r="D30" t="s">
         <v>56</v>
       </c>
-      <c r="F30" t="s">
-        <v>34</v>
-      </c>
       <c r="G30" t="s">
         <v>203</v>
       </c>
@@ -2249,9 +2237,6 @@
       </c>
       <c r="D31" t="s">
         <v>56</v>
-      </c>
-      <c r="F31" t="s">
-        <v>34</v>
       </c>
       <c r="G31" t="s">
         <v>203</v>

</xml_diff>